<commit_message>
changed RTC_REFIN to GPIO, we arent using RTC_REFIN
</commit_message>
<xml_diff>
--- a/Marionette_connections.xlsx
+++ b/Marionette_connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="400" activeTab="1"/>
+    <workbookView xWindow="2100" yWindow="21820" windowWidth="10520" windowHeight="16280" tabRatio="400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configs" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Output to ECoD" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">PinFunctions!$A:$Z</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PinFunctions!$A:$Z</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -1149,7 +1149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1428,143 +1428,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <sz val="12"/>
@@ -6794,23 +6666,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="660" activePane="bottomLeft"/>
-      <selection activeCell="O1" sqref="D1:O1048576"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="660" topLeftCell="A114" activePane="bottomLeft"/>
+      <selection sqref="A1:S1048576"/>
+      <selection pane="bottomLeft" activeCell="Y127" sqref="Y127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="32"/>
-    <col min="2" max="2" width="8.83203125" style="33"/>
-    <col min="3" max="3" width="8.83203125" style="32"/>
-    <col min="4" max="4" width="0" style="34" hidden="1" customWidth="1"/>
-    <col min="5" max="15" width="0" style="32" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="32"/>
-    <col min="17" max="22" width="0" style="32" hidden="1" customWidth="1"/>
-    <col min="23" max="24" width="0" style="34" hidden="1" customWidth="1"/>
-    <col min="25" max="1025" width="8.83203125" style="32"/>
+    <col min="2" max="2" width="8.83203125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="34" customWidth="1"/>
+    <col min="5" max="22" width="8.83203125" style="32" customWidth="1"/>
+    <col min="23" max="24" width="8.83203125" style="34" customWidth="1"/>
+    <col min="25" max="25" width="15.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="26" max="1025" width="8.83203125" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -8564,7 +8435,7 @@
       <c r="W17" s="73"/>
       <c r="X17" s="74"/>
       <c r="Y17" s="76" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="58" customFormat="1">
@@ -8698,20 +8569,18 @@
     </row>
     <row r="21" spans="1:26" s="58" customFormat="1">
       <c r="A21" s="59">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="B21" s="60" t="s">
         <v>134</v>
       </c>
       <c r="C21" s="14">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D21" s="61"/>
       <c r="E21" s="62"/>
       <c r="F21" s="62"/>
-      <c r="G21" s="62" t="s">
-        <v>145</v>
-      </c>
+      <c r="G21" s="62"/>
       <c r="H21" s="62"/>
       <c r="I21" s="62"/>
       <c r="J21" s="62"/>
@@ -8720,14 +8589,12 @@
       <c r="M21" s="62"/>
       <c r="N21" s="62"/>
       <c r="O21" s="62" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="P21" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q21" s="62" t="s">
-        <v>78</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="Q21" s="62"/>
       <c r="R21" s="62"/>
       <c r="S21" s="62"/>
       <c r="T21" s="62"/>
@@ -8735,8 +8602,8 @@
       <c r="V21" s="62"/>
       <c r="W21" s="62"/>
       <c r="X21" s="63"/>
-      <c r="Y21" s="81" t="s">
-        <v>67</v>
+      <c r="Y21" s="97" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="58" customFormat="1">
@@ -8994,20 +8861,18 @@
     </row>
     <row r="28" spans="1:26" s="58" customFormat="1">
       <c r="A28" s="59">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B28" s="60" t="s">
         <v>134</v>
       </c>
       <c r="C28" s="14">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D28" s="61"/>
       <c r="E28" s="62"/>
       <c r="F28" s="62"/>
-      <c r="G28" s="62" t="s">
-        <v>143</v>
-      </c>
+      <c r="G28" s="62"/>
       <c r="H28" s="62"/>
       <c r="I28" s="62"/>
       <c r="J28" s="62"/>
@@ -9016,14 +8881,12 @@
       <c r="M28" s="62"/>
       <c r="N28" s="62"/>
       <c r="O28" s="62" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="P28" s="62" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q28" s="62" t="s">
-        <v>72</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="Q28" s="62"/>
       <c r="R28" s="62"/>
       <c r="S28" s="62"/>
       <c r="T28" s="62"/>
@@ -9031,8 +8894,8 @@
       <c r="V28" s="62"/>
       <c r="W28" s="62"/>
       <c r="X28" s="63"/>
-      <c r="Y28" s="81" t="s">
-        <v>77</v>
+      <c r="Y28" s="97" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:26" s="58" customFormat="1">
@@ -9122,21 +8985,23 @@
     </row>
     <row r="31" spans="1:26" s="58" customFormat="1">
       <c r="A31" s="59">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="B31" s="60" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="C31" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="61"/>
       <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="H31" s="62"/>
+      <c r="F31" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62" t="s">
+        <v>138</v>
+      </c>
       <c r="I31" s="62"/>
       <c r="J31" s="62"/>
       <c r="K31" s="62"/>
@@ -9144,23 +9009,21 @@
       <c r="M31" s="62"/>
       <c r="N31" s="62"/>
       <c r="O31" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="P31" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q31" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="R31" s="62"/>
+        <v>82</v>
+      </c>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62" t="s">
+        <v>175</v>
+      </c>
       <c r="S31" s="62"/>
       <c r="T31" s="62"/>
       <c r="U31" s="62"/>
       <c r="V31" s="62"/>
       <c r="W31" s="62"/>
       <c r="X31" s="63"/>
-      <c r="Y31" s="81" t="s">
-        <v>75</v>
+      <c r="Y31" s="97" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:26" s="58" customFormat="1">
@@ -9202,10 +9065,10 @@
     </row>
     <row r="33" spans="1:25" s="58" customFormat="1">
       <c r="A33" s="70">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="B33" s="71" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="C33" s="31">
         <v>8</v>
@@ -9214,29 +9077,33 @@
       <c r="E33" s="73"/>
       <c r="F33" s="73"/>
       <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
+      <c r="H33" s="73" t="s">
+        <v>139</v>
+      </c>
       <c r="I33" s="73"/>
       <c r="J33" s="73"/>
       <c r="K33" s="73"/>
       <c r="L33" s="73"/>
       <c r="M33" s="73"/>
-      <c r="N33" s="73"/>
+      <c r="N33" s="73" t="s">
+        <v>132</v>
+      </c>
       <c r="O33" s="73" t="s">
-        <v>71</v>
-      </c>
-      <c r="P33" s="73" t="s">
-        <v>180</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="P33" s="73"/>
       <c r="Q33" s="73"/>
-      <c r="R33" s="73"/>
+      <c r="R33" s="73" t="s">
+        <v>135</v>
+      </c>
       <c r="S33" s="73"/>
       <c r="T33" s="73"/>
       <c r="U33" s="73"/>
       <c r="V33" s="73"/>
       <c r="W33" s="73"/>
       <c r="X33" s="74"/>
-      <c r="Y33" s="81" t="s">
-        <v>71</v>
+      <c r="Y33" s="97" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:25" s="58" customFormat="1">
@@ -9395,18 +9262,20 @@
     </row>
     <row r="38" spans="1:25" s="58" customFormat="1">
       <c r="A38" s="59">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B38" s="60" t="s">
         <v>134</v>
       </c>
       <c r="C38" s="14">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D38" s="61"/>
       <c r="E38" s="62"/>
       <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
+      <c r="G38" s="62" t="s">
+        <v>143</v>
+      </c>
       <c r="H38" s="62"/>
       <c r="I38" s="62"/>
       <c r="J38" s="62"/>
@@ -9415,12 +9284,14 @@
       <c r="M38" s="62"/>
       <c r="N38" s="62"/>
       <c r="O38" s="62" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="P38" s="62" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q38" s="62"/>
+        <v>170</v>
+      </c>
+      <c r="Q38" s="62" t="s">
+        <v>72</v>
+      </c>
       <c r="R38" s="62"/>
       <c r="S38" s="62"/>
       <c r="T38" s="62"/>
@@ -9429,7 +9300,7 @@
       <c r="W38" s="62"/>
       <c r="X38" s="63"/>
       <c r="Y38" s="81" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:25" s="58" customFormat="1">
@@ -9471,18 +9342,20 @@
     </row>
     <row r="40" spans="1:25" s="58" customFormat="1">
       <c r="A40" s="59">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B40" s="60" t="s">
         <v>134</v>
       </c>
       <c r="C40" s="14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D40" s="61"/>
       <c r="E40" s="62"/>
       <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
+      <c r="G40" s="62" t="s">
+        <v>159</v>
+      </c>
       <c r="H40" s="62"/>
       <c r="I40" s="62"/>
       <c r="J40" s="62"/>
@@ -9491,12 +9364,14 @@
       <c r="M40" s="62"/>
       <c r="N40" s="62"/>
       <c r="O40" s="62" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="P40" s="62" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q40" s="62"/>
+        <v>168</v>
+      </c>
+      <c r="Q40" s="62" t="s">
+        <v>74</v>
+      </c>
       <c r="R40" s="62"/>
       <c r="S40" s="62"/>
       <c r="T40" s="62"/>
@@ -9505,7 +9380,7 @@
       <c r="W40" s="62"/>
       <c r="X40" s="63"/>
       <c r="Y40" s="81" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:25" s="58" customFormat="1">
@@ -12597,7 +12472,7 @@
       <c r="W126" s="62"/>
       <c r="X126" s="63"/>
       <c r="Y126" s="68" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:25">
@@ -13648,13 +13523,13 @@
     </row>
     <row r="157" spans="1:25">
       <c r="A157" s="59">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="B157" s="60" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="C157" s="14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D157" s="61"/>
       <c r="E157" s="62"/>
@@ -13668,9 +13543,11 @@
       <c r="M157" s="62"/>
       <c r="N157" s="62"/>
       <c r="O157" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="P157" s="62"/>
+        <v>71</v>
+      </c>
+      <c r="P157" s="62" t="s">
+        <v>180</v>
+      </c>
       <c r="Q157" s="62"/>
       <c r="R157" s="62"/>
       <c r="S157" s="62"/>
@@ -13680,7 +13557,7 @@
       <c r="W157" s="62"/>
       <c r="X157" s="63"/>
       <c r="Y157" s="81" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="158" spans="1:25">
@@ -14043,37 +13920,31 @@
     </row>
     <row r="168" spans="1:25">
       <c r="A168" s="59">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="B168" s="60" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="C168" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D168" s="61"/>
       <c r="E168" s="62"/>
       <c r="F168" s="62"/>
       <c r="G168" s="62"/>
-      <c r="H168" s="62" t="s">
-        <v>139</v>
-      </c>
+      <c r="H168" s="62"/>
       <c r="I168" s="62"/>
       <c r="J168" s="62"/>
       <c r="K168" s="62"/>
       <c r="L168" s="62"/>
       <c r="M168" s="62"/>
-      <c r="N168" s="62" t="s">
-        <v>132</v>
-      </c>
+      <c r="N168" s="62"/>
       <c r="O168" s="62" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="P168" s="62"/>
       <c r="Q168" s="62"/>
-      <c r="R168" s="62" t="s">
-        <v>135</v>
-      </c>
+      <c r="R168" s="62"/>
       <c r="S168" s="62"/>
       <c r="T168" s="62"/>
       <c r="U168" s="62"/>
@@ -14081,28 +13952,26 @@
       <c r="W168" s="62"/>
       <c r="X168" s="63"/>
       <c r="Y168" s="81" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="169" spans="1:25">
       <c r="A169" s="59">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B169" s="60" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="C169" s="14">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D169" s="61"/>
       <c r="E169" s="62"/>
-      <c r="F169" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="G169" s="62"/>
-      <c r="H169" s="62" t="s">
-        <v>138</v>
-      </c>
+      <c r="F169" s="62"/>
+      <c r="G169" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="H169" s="62"/>
       <c r="I169" s="62"/>
       <c r="J169" s="62"/>
       <c r="K169" s="62"/>
@@ -14110,13 +13979,15 @@
       <c r="M169" s="62"/>
       <c r="N169" s="62"/>
       <c r="O169" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="P169" s="62"/>
-      <c r="Q169" s="62"/>
-      <c r="R169" s="62" t="s">
-        <v>175</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="P169" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q169" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="R169" s="62"/>
       <c r="S169" s="62"/>
       <c r="T169" s="62"/>
       <c r="U169" s="62"/>
@@ -14124,7 +13995,7 @@
       <c r="W169" s="62"/>
       <c r="X169" s="63"/>
       <c r="Y169" s="81" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="170" spans="1:25">
@@ -14401,8 +14272,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Z1048576">
-    <sortState ref="A2:Z177">
-      <sortCondition ref="P1:P1048576"/>
+    <sortState ref="A21:Z169">
+      <sortCondition descending="1" ref="Y1:Y1048576"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Selected USART pins to drive external DAC
</commit_message>
<xml_diff>
--- a/Marionette_connections.xlsx
+++ b/Marionette_connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="21820" windowWidth="10520" windowHeight="16280" tabRatio="400" activeTab="1"/>
+    <workbookView xWindow="2100" yWindow="21820" windowWidth="22540" windowHeight="16880" tabRatio="400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="233">
   <si>
     <t>Pin number</t>
   </si>
@@ -721,6 +721,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>USART_CK</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +860,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF93CDDD"/>
         <bgColor rgb="FFB9CDE5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1149,7 +1158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1429,6 +1438,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -6664,22 +6677,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AMK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="660" topLeftCell="A114" activePane="bottomLeft"/>
-      <selection sqref="A1:S1048576"/>
-      <selection pane="bottomLeft" activeCell="Y127" sqref="Y127"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="660" activePane="bottomLeft"/>
+      <selection activeCell="Q1" sqref="Q1:X1048576"/>
+      <selection pane="bottomLeft" activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="32"/>
     <col min="2" max="2" width="8.83203125" style="33" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="34" customWidth="1"/>
-    <col min="5" max="22" width="8.83203125" style="32" customWidth="1"/>
-    <col min="23" max="24" width="8.83203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="34" hidden="1" customWidth="1"/>
+    <col min="5" max="15" width="8.83203125" style="32" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="32" customWidth="1"/>
+    <col min="17" max="22" width="8.83203125" style="32" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="8.83203125" style="34" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="15.5" style="32" bestFit="1" customWidth="1"/>
     <col min="26" max="1025" width="8.83203125" style="32"/>
   </cols>
@@ -7760,7 +7776,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="58" customFormat="1">
+    <row r="2" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A2" s="52">
         <v>119</v>
       </c>
@@ -7803,7 +7819,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" s="58" customFormat="1">
+    <row r="3" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A3" s="59">
         <v>122</v>
       </c>
@@ -7844,7 +7860,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="58" customFormat="1">
+    <row r="4" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A4" s="59">
         <v>123</v>
       </c>
@@ -7885,7 +7901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" s="58" customFormat="1">
+    <row r="5" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A5" s="59">
         <v>121</v>
       </c>
@@ -7924,7 +7940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" s="58" customFormat="1">
+    <row r="6" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A6" s="59">
         <v>165</v>
       </c>
@@ -7963,7 +7979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" s="58" customFormat="1">
+    <row r="7" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A7" s="59">
         <v>120</v>
       </c>
@@ -8002,7 +8018,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:1024" s="58" customFormat="1">
+    <row r="8" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A8" s="59">
         <v>164</v>
       </c>
@@ -8043,7 +8059,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" s="58" customFormat="1">
+    <row r="9" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A9" s="59">
         <v>50</v>
       </c>
@@ -8092,13 +8108,13 @@
     </row>
     <row r="10" spans="1:1024" s="58" customFormat="1">
       <c r="A10" s="59">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B10" s="60" t="s">
         <v>179</v>
       </c>
       <c r="C10" s="14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" s="61"/>
       <c r="E10" s="62"/>
@@ -8113,7 +8129,7 @@
       <c r="N10" s="62"/>
       <c r="O10" s="62"/>
       <c r="P10" s="62" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q10" s="62"/>
       <c r="R10" s="62"/>
@@ -8123,14 +8139,14 @@
       <c r="V10" s="62"/>
       <c r="W10" s="62"/>
       <c r="X10" s="63"/>
-      <c r="Y10" s="64" t="s">
-        <v>18</v>
+      <c r="Y10" s="98" t="s">
+        <v>154</v>
       </c>
       <c r="Z10" s="58" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:1024" s="58" customFormat="1">
+    <row r="11" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A11" s="59">
         <v>40</v>
       </c>
@@ -8177,7 +8193,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" s="58" customFormat="1">
+    <row r="12" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A12" s="59">
         <v>145</v>
       </c>
@@ -8217,7 +8233,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" s="58" customFormat="1">
+    <row r="13" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A13" s="59">
         <v>41</v>
       </c>
@@ -8266,7 +8282,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" s="58" customFormat="1">
+    <row r="14" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A14" s="59">
         <v>146</v>
       </c>
@@ -8306,7 +8322,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:1024" s="58" customFormat="1">
+    <row r="15" spans="1:1024" s="58" customFormat="1" hidden="1">
       <c r="A15" s="59">
         <v>47</v>
       </c>
@@ -8386,14 +8402,14 @@
       <c r="V16" s="62"/>
       <c r="W16" s="62"/>
       <c r="X16" s="63"/>
-      <c r="Y16" s="68" t="s">
-        <v>18</v>
+      <c r="Y16" s="98" t="s">
+        <v>156</v>
       </c>
       <c r="Z16" s="58" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="58" customFormat="1">
+    <row r="17" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A17" s="70">
         <v>42</v>
       </c>
@@ -8440,13 +8456,13 @@
     </row>
     <row r="18" spans="1:26" s="58" customFormat="1">
       <c r="A18" s="52">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>179</v>
       </c>
       <c r="C18" s="17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D18" s="54"/>
       <c r="E18" s="55"/>
@@ -8461,7 +8477,7 @@
       <c r="N18" s="55"/>
       <c r="O18" s="55"/>
       <c r="P18" s="55" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="Q18" s="55"/>
       <c r="R18" s="55"/>
@@ -8471,14 +8487,14 @@
       <c r="V18" s="55"/>
       <c r="W18" s="55"/>
       <c r="X18" s="56"/>
-      <c r="Y18" s="68" t="s">
-        <v>18</v>
+      <c r="Y18" s="98" t="s">
+        <v>232</v>
       </c>
       <c r="Z18" s="58" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="58" customFormat="1">
+    <row r="19" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A19" s="59">
         <v>92</v>
       </c>
@@ -8527,15 +8543,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:26" s="58" customFormat="1">
+    <row r="20" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A20" s="59">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C20" s="14">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D20" s="61"/>
       <c r="E20" s="62"/>
@@ -8550,7 +8566,7 @@
       <c r="N20" s="62"/>
       <c r="O20" s="62"/>
       <c r="P20" s="62" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="Q20" s="62"/>
       <c r="R20" s="62"/>
@@ -8563,11 +8579,8 @@
       <c r="Y20" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="Z20" s="58" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" s="58" customFormat="1">
+    </row>
+    <row r="21" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A21" s="59">
         <v>116</v>
       </c>
@@ -8606,7 +8619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="58" customFormat="1">
+    <row r="22" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A22" s="59">
         <v>93</v>
       </c>
@@ -8653,7 +8666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="58" customFormat="1">
+    <row r="23" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A23" s="59">
         <v>99</v>
       </c>
@@ -8693,7 +8706,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="58" customFormat="1">
+    <row r="24" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A24" s="59">
         <v>94</v>
       </c>
@@ -8734,7 +8747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="58" customFormat="1">
+    <row r="25" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A25" s="59">
         <v>100</v>
       </c>
@@ -8774,7 +8787,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="58" customFormat="1">
+    <row r="26" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A26" s="59">
         <v>80</v>
       </c>
@@ -8821,13 +8834,13 @@
     </row>
     <row r="27" spans="1:26" s="58" customFormat="1">
       <c r="A27" s="59">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" s="60" t="s">
         <v>179</v>
       </c>
       <c r="C27" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="62"/>
@@ -8842,7 +8855,7 @@
       <c r="N27" s="62"/>
       <c r="O27" s="62"/>
       <c r="P27" s="62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q27" s="62"/>
       <c r="R27" s="62"/>
@@ -8852,14 +8865,14 @@
       <c r="V27" s="62"/>
       <c r="W27" s="62"/>
       <c r="X27" s="63"/>
-      <c r="Y27" s="68" t="s">
+      <c r="Y27" s="97" t="s">
         <v>18</v>
       </c>
       <c r="Z27" s="58" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="58" customFormat="1">
+    <row r="28" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A28" s="59">
         <v>115</v>
       </c>
@@ -8898,7 +8911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="58" customFormat="1">
+    <row r="29" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A29" s="59">
         <v>79</v>
       </c>
@@ -8945,13 +8958,13 @@
     </row>
     <row r="30" spans="1:26" s="58" customFormat="1">
       <c r="A30" s="59">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B30" s="60" t="s">
         <v>179</v>
       </c>
       <c r="C30" s="14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D30" s="61"/>
       <c r="E30" s="62"/>
@@ -8966,7 +8979,7 @@
       <c r="N30" s="62"/>
       <c r="O30" s="62"/>
       <c r="P30" s="62" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q30" s="62"/>
       <c r="R30" s="62"/>
@@ -8983,7 +8996,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="58" customFormat="1">
+    <row r="31" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A31" s="59">
         <v>168</v>
       </c>
@@ -9026,15 +9039,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:26" s="58" customFormat="1">
+    <row r="32" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A32" s="59">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="B32" s="60" t="s">
         <v>167</v>
       </c>
       <c r="C32" s="14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D32" s="61"/>
       <c r="E32" s="62"/>
@@ -9049,7 +9062,7 @@
       <c r="N32" s="62"/>
       <c r="O32" s="62"/>
       <c r="P32" s="62" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="Q32" s="62"/>
       <c r="R32" s="62"/>
@@ -9063,7 +9076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="58" customFormat="1">
+    <row r="33" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A33" s="70">
         <v>167</v>
       </c>
@@ -9106,7 +9119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="58" customFormat="1">
+    <row r="34" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A34" s="52">
         <v>156</v>
       </c>
@@ -9147,7 +9160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:25" s="58" customFormat="1">
+    <row r="35" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A35" s="59">
         <v>160</v>
       </c>
@@ -9184,7 +9197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="58" customFormat="1">
+    <row r="36" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A36" s="59">
         <v>112</v>
       </c>
@@ -9223,7 +9236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="58" customFormat="1">
+    <row r="37" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A37" s="59">
         <v>155</v>
       </c>
@@ -9260,7 +9273,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="58" customFormat="1">
+    <row r="38" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A38" s="59">
         <v>140</v>
       </c>
@@ -9303,15 +9316,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="58" customFormat="1">
+    <row r="39" spans="1:26" s="58" customFormat="1">
       <c r="A39" s="59">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="B39" s="60" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="C39" s="14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D39" s="61"/>
       <c r="E39" s="62"/>
@@ -9326,7 +9339,7 @@
       <c r="N39" s="62"/>
       <c r="O39" s="62"/>
       <c r="P39" s="62" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="Q39" s="62"/>
       <c r="R39" s="62"/>
@@ -9339,8 +9352,11 @@
       <c r="Y39" s="68" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" s="58" customFormat="1">
+      <c r="Z39" s="58" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A40" s="59">
         <v>139</v>
       </c>
@@ -9383,7 +9399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="58" customFormat="1">
+    <row r="41" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A41" s="59">
         <v>157</v>
       </c>
@@ -9424,7 +9440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:25" s="58" customFormat="1">
+    <row r="42" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A42" s="59">
         <v>1</v>
       </c>
@@ -9461,7 +9477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="58" customFormat="1">
+    <row r="43" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A43" s="59">
         <v>2</v>
       </c>
@@ -9496,7 +9512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="58" customFormat="1">
+    <row r="44" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A44" s="59">
         <v>3</v>
       </c>
@@ -9531,7 +9547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="58" customFormat="1">
+    <row r="45" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A45" s="59">
         <v>4</v>
       </c>
@@ -9566,7 +9582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="58" customFormat="1">
+    <row r="46" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A46" s="59">
         <v>5</v>
       </c>
@@ -9601,7 +9617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:25" s="58" customFormat="1">
+    <row r="47" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A47" s="59">
         <v>6</v>
       </c>
@@ -9632,7 +9648,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="58" customFormat="1">
+    <row r="48" spans="1:26" s="58" customFormat="1" hidden="1">
       <c r="A48" s="59">
         <v>7</v>
       </c>
@@ -9667,7 +9683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="58" customFormat="1">
+    <row r="49" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A49" s="70">
         <v>8</v>
       </c>
@@ -9702,7 +9718,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="58" customFormat="1">
+    <row r="50" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A50" s="52">
         <v>9</v>
       </c>
@@ -9737,7 +9753,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="58" customFormat="1">
+    <row r="51" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A51" s="59">
         <v>10</v>
       </c>
@@ -9772,7 +9788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="58" customFormat="1">
+    <row r="52" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A52" s="59">
         <v>11</v>
       </c>
@@ -9809,7 +9825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="58" customFormat="1">
+    <row r="53" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A53" s="59">
         <v>12</v>
       </c>
@@ -9846,7 +9862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="58" customFormat="1">
+    <row r="54" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A54" s="59">
         <v>13</v>
       </c>
@@ -9883,7 +9899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="58" customFormat="1">
+    <row r="55" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A55" s="59">
         <v>14</v>
       </c>
@@ -9914,7 +9930,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="58" customFormat="1">
+    <row r="56" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A56" s="59">
         <v>15</v>
       </c>
@@ -9945,7 +9961,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="58" customFormat="1">
+    <row r="57" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A57" s="59">
         <v>16</v>
       </c>
@@ -9982,7 +9998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:25" s="58" customFormat="1">
+    <row r="58" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A58" s="59">
         <v>17</v>
       </c>
@@ -10019,7 +10035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="58" customFormat="1">
+    <row r="59" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A59" s="59">
         <v>18</v>
       </c>
@@ -10056,7 +10072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:25" s="58" customFormat="1">
+    <row r="60" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A60" s="59">
         <v>19</v>
       </c>
@@ -10093,7 +10109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:25" s="58" customFormat="1">
+    <row r="61" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A61" s="59">
         <v>20</v>
       </c>
@@ -10130,7 +10146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="58" customFormat="1">
+    <row r="62" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A62" s="59">
         <v>21</v>
       </c>
@@ -10167,7 +10183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="58" customFormat="1">
+    <row r="63" spans="1:25" s="58" customFormat="1" hidden="1">
       <c r="A63" s="59">
         <v>22</v>
       </c>
@@ -10198,7 +10214,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" hidden="1">
       <c r="A64" s="59">
         <v>23</v>
       </c>
@@ -10229,7 +10245,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" hidden="1">
       <c r="A65" s="70">
         <v>24</v>
       </c>
@@ -10266,7 +10282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" hidden="1">
       <c r="A66" s="52">
         <v>25</v>
       </c>
@@ -10303,7 +10319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" hidden="1">
       <c r="A67" s="59">
         <v>26</v>
       </c>
@@ -10340,7 +10356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" hidden="1">
       <c r="A68" s="59">
         <v>27</v>
       </c>
@@ -10377,7 +10393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" hidden="1">
       <c r="A69" s="59">
         <v>28</v>
       </c>
@@ -10414,7 +10430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" hidden="1">
       <c r="A70" s="59">
         <v>29</v>
       </c>
@@ -10449,7 +10465,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" hidden="1">
       <c r="A71" s="59">
         <v>30</v>
       </c>
@@ -10484,7 +10500,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" hidden="1">
       <c r="A72" s="59">
         <v>31</v>
       </c>
@@ -10515,7 +10531,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" hidden="1">
       <c r="A73" s="59">
         <v>32</v>
       </c>
@@ -10558,7 +10574,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" hidden="1">
       <c r="A74" s="59">
         <v>33</v>
       </c>
@@ -10601,7 +10617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" hidden="1">
       <c r="A75" s="59">
         <v>34</v>
       </c>
@@ -10648,7 +10664,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" hidden="1">
       <c r="A76" s="59">
         <v>35</v>
       </c>
@@ -10695,7 +10711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" hidden="1">
       <c r="A77" s="59">
         <v>36</v>
       </c>
@@ -10726,7 +10742,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" hidden="1">
       <c r="A78" s="59">
         <v>37</v>
       </c>
@@ -10757,7 +10773,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" hidden="1">
       <c r="A79" s="59">
         <v>38</v>
       </c>
@@ -10788,7 +10804,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" hidden="1">
       <c r="A80" s="59">
         <v>39</v>
       </c>
@@ -10819,7 +10835,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:25" hidden="1">
       <c r="A81" s="70">
         <v>43</v>
       </c>
@@ -10856,7 +10872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:25">
+    <row r="82" spans="1:25" hidden="1">
       <c r="A82" s="52">
         <v>44</v>
       </c>
@@ -10893,7 +10909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" hidden="1">
       <c r="A83" s="59">
         <v>45</v>
       </c>
@@ -10932,7 +10948,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:25" hidden="1">
       <c r="A84" s="59">
         <v>46</v>
       </c>
@@ -10969,7 +10985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" hidden="1">
       <c r="A85" s="59">
         <v>48</v>
       </c>
@@ -11000,7 +11016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" hidden="1">
       <c r="A86" s="59">
         <v>49</v>
       </c>
@@ -11031,7 +11047,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" hidden="1">
       <c r="A87" s="59">
         <v>51</v>
       </c>
@@ -11076,7 +11092,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" hidden="1">
       <c r="A88" s="59">
         <v>52</v>
       </c>
@@ -11117,7 +11133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" hidden="1">
       <c r="A89" s="59">
         <v>53</v>
       </c>
@@ -11162,7 +11178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" hidden="1">
       <c r="A90" s="59">
         <v>54</v>
       </c>
@@ -11205,7 +11221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:25" hidden="1">
       <c r="A91" s="59">
         <v>55</v>
       </c>
@@ -11248,7 +11264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:25">
+    <row r="92" spans="1:25" hidden="1">
       <c r="A92" s="59">
         <v>56</v>
       </c>
@@ -11291,7 +11307,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:25">
+    <row r="93" spans="1:25" hidden="1">
       <c r="A93" s="59">
         <v>57</v>
       </c>
@@ -11334,7 +11350,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:25">
+    <row r="94" spans="1:25" hidden="1">
       <c r="A94" s="59">
         <v>58</v>
       </c>
@@ -11369,7 +11385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:25">
+    <row r="95" spans="1:25" hidden="1">
       <c r="A95" s="59">
         <v>59</v>
       </c>
@@ -11404,7 +11420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:25">
+    <row r="96" spans="1:25" hidden="1">
       <c r="A96" s="59">
         <v>60</v>
       </c>
@@ -11439,7 +11455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:25">
+    <row r="97" spans="1:25" hidden="1">
       <c r="A97" s="70">
         <v>61</v>
       </c>
@@ -11470,7 +11486,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="98" spans="1:25">
+    <row r="98" spans="1:25" hidden="1">
       <c r="A98" s="52">
         <v>62</v>
       </c>
@@ -11501,7 +11517,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:25">
+    <row r="99" spans="1:25" hidden="1">
       <c r="A99" s="59">
         <v>63</v>
       </c>
@@ -11536,7 +11552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:25">
+    <row r="100" spans="1:25" hidden="1">
       <c r="A100" s="59">
         <v>64</v>
       </c>
@@ -11571,7 +11587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:25">
+    <row r="101" spans="1:25" hidden="1">
       <c r="A101" s="59">
         <v>65</v>
       </c>
@@ -11606,7 +11622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:25">
+    <row r="102" spans="1:25" hidden="1">
       <c r="A102" s="59">
         <v>66</v>
       </c>
@@ -11641,7 +11657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:25">
+    <row r="103" spans="1:25" hidden="1">
       <c r="A103" s="59">
         <v>67</v>
       </c>
@@ -11676,7 +11692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:25">
+    <row r="104" spans="1:25" hidden="1">
       <c r="A104" s="59">
         <v>68</v>
       </c>
@@ -11711,7 +11727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:25">
+    <row r="105" spans="1:25" hidden="1">
       <c r="A105" s="59">
         <v>69</v>
       </c>
@@ -11746,7 +11762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:25">
+    <row r="106" spans="1:25" hidden="1">
       <c r="A106" s="59">
         <v>70</v>
       </c>
@@ -11781,7 +11797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:25" hidden="1">
       <c r="A107" s="59">
         <v>71</v>
       </c>
@@ -11812,7 +11828,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:25">
+    <row r="108" spans="1:25" hidden="1">
       <c r="A108" s="59">
         <v>72</v>
       </c>
@@ -11843,7 +11859,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:25">
+    <row r="109" spans="1:25" hidden="1">
       <c r="A109" s="59">
         <v>73</v>
       </c>
@@ -11878,7 +11894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:25">
+    <row r="110" spans="1:25" hidden="1">
       <c r="A110" s="59">
         <v>74</v>
       </c>
@@ -11913,7 +11929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:25">
+    <row r="111" spans="1:25" hidden="1">
       <c r="A111" s="59">
         <v>75</v>
       </c>
@@ -11948,7 +11964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:25">
+    <row r="112" spans="1:25" hidden="1">
       <c r="A112" s="59">
         <v>76</v>
       </c>
@@ -11983,7 +11999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:25">
+    <row r="113" spans="1:25" hidden="1">
       <c r="A113" s="70">
         <v>77</v>
       </c>
@@ -12018,7 +12034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:25">
+    <row r="114" spans="1:25" hidden="1">
       <c r="A114" s="52">
         <v>78</v>
       </c>
@@ -12053,7 +12069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:25">
+    <row r="115" spans="1:25" hidden="1">
       <c r="A115" s="59">
         <v>81</v>
       </c>
@@ -12084,7 +12100,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="116" spans="1:25">
+    <row r="116" spans="1:25" hidden="1">
       <c r="A116" s="59">
         <v>82</v>
       </c>
@@ -12115,7 +12131,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="117" spans="1:25">
+    <row r="117" spans="1:25" hidden="1">
       <c r="A117" s="59">
         <v>83</v>
       </c>
@@ -12154,7 +12170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:25">
+    <row r="118" spans="1:25" hidden="1">
       <c r="A118" s="59">
         <v>84</v>
       </c>
@@ -12193,7 +12209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:25">
+    <row r="119" spans="1:25" hidden="1">
       <c r="A119" s="59">
         <v>85</v>
       </c>
@@ -12230,7 +12246,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:25">
+    <row r="120" spans="1:25" hidden="1">
       <c r="A120" s="59">
         <v>86</v>
       </c>
@@ -12267,7 +12283,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:25">
+    <row r="121" spans="1:25" hidden="1">
       <c r="A121" s="59">
         <v>87</v>
       </c>
@@ -12302,7 +12318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:25">
+    <row r="122" spans="1:25" hidden="1">
       <c r="A122" s="59">
         <v>88</v>
       </c>
@@ -12337,7 +12353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:25">
+    <row r="123" spans="1:25" hidden="1">
       <c r="A123" s="59">
         <v>89</v>
       </c>
@@ -12372,7 +12388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:25">
+    <row r="124" spans="1:25" hidden="1">
       <c r="A124" s="59">
         <v>90</v>
       </c>
@@ -12403,7 +12419,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="125" spans="1:25">
+    <row r="125" spans="1:25" hidden="1">
       <c r="A125" s="59">
         <v>91</v>
       </c>
@@ -12434,7 +12450,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="126" spans="1:25">
+    <row r="126" spans="1:25" hidden="1">
       <c r="A126" s="59">
         <v>95</v>
       </c>
@@ -12475,7 +12491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:25">
+    <row r="127" spans="1:25" hidden="1">
       <c r="A127" s="59">
         <v>101</v>
       </c>
@@ -12510,7 +12526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:25">
+    <row r="128" spans="1:25" hidden="1">
       <c r="A128" s="59">
         <v>102</v>
       </c>
@@ -12541,7 +12557,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="129" spans="1:25">
+    <row r="129" spans="1:25" hidden="1">
       <c r="A129" s="70">
         <v>103</v>
       </c>
@@ -12572,7 +12588,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" hidden="1">
       <c r="A130" s="83">
         <v>104</v>
       </c>
@@ -12607,7 +12623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:25">
+    <row r="131" spans="1:25" hidden="1">
       <c r="A131" s="59">
         <v>105</v>
       </c>
@@ -12642,7 +12658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:25">
+    <row r="132" spans="1:25" hidden="1">
       <c r="A132" s="59">
         <v>106</v>
       </c>
@@ -12677,7 +12693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:25">
+    <row r="133" spans="1:25" hidden="1">
       <c r="A133" s="59">
         <v>107</v>
       </c>
@@ -12712,7 +12728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:25">
+    <row r="134" spans="1:25" hidden="1">
       <c r="A134" s="59">
         <v>108</v>
       </c>
@@ -12747,7 +12763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" hidden="1">
       <c r="A135" s="59">
         <v>109</v>
       </c>
@@ -12782,7 +12798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:25">
+    <row r="136" spans="1:25" hidden="1">
       <c r="A136" s="59">
         <v>110</v>
       </c>
@@ -12817,7 +12833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:25">
+    <row r="137" spans="1:25" hidden="1">
       <c r="A137" s="59">
         <v>113</v>
       </c>
@@ -12848,7 +12864,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="138" spans="1:25">
+    <row r="138" spans="1:25" hidden="1">
       <c r="A138" s="59">
         <v>114</v>
       </c>
@@ -12879,7 +12895,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="139" spans="1:25">
+    <row r="139" spans="1:25" hidden="1">
       <c r="A139" s="59">
         <v>118</v>
       </c>
@@ -12920,7 +12936,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" hidden="1">
       <c r="A140" s="59">
         <v>124</v>
       </c>
@@ -12957,7 +12973,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="1:25">
+    <row r="141" spans="1:25" hidden="1">
       <c r="A141" s="59">
         <v>125</v>
       </c>
@@ -12988,7 +13004,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="142" spans="1:25">
+    <row r="142" spans="1:25" hidden="1">
       <c r="A142" s="59">
         <v>126</v>
       </c>
@@ -13019,7 +13035,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="143" spans="1:25">
+    <row r="143" spans="1:25" hidden="1">
       <c r="A143" s="59">
         <v>127</v>
       </c>
@@ -13050,7 +13066,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="144" spans="1:25">
+    <row r="144" spans="1:25" hidden="1">
       <c r="A144" s="59">
         <v>128</v>
       </c>
@@ -13087,7 +13103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" spans="1:25">
+    <row r="145" spans="1:25" hidden="1">
       <c r="A145" s="59">
         <v>129</v>
       </c>
@@ -13122,7 +13138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:25">
+    <row r="146" spans="1:25" hidden="1">
       <c r="A146" s="59">
         <v>130</v>
       </c>
@@ -13157,7 +13173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:25">
+    <row r="147" spans="1:25" hidden="1">
       <c r="A147" s="59">
         <v>131</v>
       </c>
@@ -13194,7 +13210,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="148" spans="1:25">
+    <row r="148" spans="1:25" hidden="1">
       <c r="A148" s="90">
         <v>132</v>
       </c>
@@ -13231,7 +13247,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="149" spans="1:25">
+    <row r="149" spans="1:25" hidden="1">
       <c r="A149" s="90">
         <v>133</v>
       </c>
@@ -13268,7 +13284,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="150" spans="1:25">
+    <row r="150" spans="1:25" hidden="1">
       <c r="A150" s="90">
         <v>134</v>
       </c>
@@ -13305,7 +13321,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:25">
+    <row r="151" spans="1:25" hidden="1">
       <c r="A151" s="59">
         <v>135</v>
       </c>
@@ -13336,7 +13352,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="152" spans="1:25">
+    <row r="152" spans="1:25" hidden="1">
       <c r="A152" s="59">
         <v>136</v>
       </c>
@@ -13367,7 +13383,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="153" spans="1:25">
+    <row r="153" spans="1:25" hidden="1">
       <c r="A153" s="59">
         <v>137</v>
       </c>
@@ -13404,7 +13420,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="154" spans="1:25">
+    <row r="154" spans="1:25" hidden="1">
       <c r="A154" s="59">
         <v>138</v>
       </c>
@@ -13445,7 +13461,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:25">
+    <row r="155" spans="1:25" hidden="1">
       <c r="A155" s="59">
         <v>142</v>
       </c>
@@ -13482,7 +13498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:25">
+    <row r="156" spans="1:25" hidden="1">
       <c r="A156" s="59">
         <v>143</v>
       </c>
@@ -13521,7 +13537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:25">
+    <row r="157" spans="1:25" hidden="1">
       <c r="A157" s="59">
         <v>117</v>
       </c>
@@ -13560,7 +13576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="158" spans="1:25">
+    <row r="158" spans="1:25" hidden="1">
       <c r="A158" s="59">
         <v>148</v>
       </c>
@@ -13591,7 +13607,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="159" spans="1:25">
+    <row r="159" spans="1:25" hidden="1">
       <c r="A159" s="59">
         <v>149</v>
       </c>
@@ -13622,7 +13638,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="160" spans="1:25">
+    <row r="160" spans="1:25" hidden="1">
       <c r="A160" s="59">
         <v>153</v>
       </c>
@@ -13657,7 +13673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:25">
+    <row r="161" spans="1:25" hidden="1">
       <c r="A161" s="59">
         <v>154</v>
       </c>
@@ -13696,7 +13712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:25">
+    <row r="162" spans="1:25" hidden="1">
       <c r="A162" s="59">
         <v>158</v>
       </c>
@@ -13727,7 +13743,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="163" spans="1:25">
+    <row r="163" spans="1:25" hidden="1">
       <c r="A163" s="59">
         <v>159</v>
       </c>
@@ -13758,7 +13774,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:25">
+    <row r="164" spans="1:25" hidden="1">
       <c r="A164" s="59">
         <v>161</v>
       </c>
@@ -13799,7 +13815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:25">
+    <row r="165" spans="1:25" hidden="1">
       <c r="A165" s="59">
         <v>162</v>
       </c>
@@ -13840,7 +13856,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:25">
+    <row r="166" spans="1:25" hidden="1">
       <c r="A166" s="59">
         <v>163</v>
       </c>
@@ -13887,7 +13903,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="167" spans="1:25">
+    <row r="167" spans="1:25" hidden="1">
       <c r="A167" s="59">
         <v>166</v>
       </c>
@@ -13918,7 +13934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:25">
+    <row r="168" spans="1:25" hidden="1">
       <c r="A168" s="59">
         <v>144</v>
       </c>
@@ -13955,7 +13971,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="169" spans="1:25">
+    <row r="169" spans="1:25" hidden="1">
       <c r="A169" s="59">
         <v>141</v>
       </c>
@@ -13998,7 +14014,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="170" spans="1:25">
+    <row r="170" spans="1:25" hidden="1">
       <c r="A170" s="59">
         <v>169</v>
       </c>
@@ -14033,7 +14049,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:25">
+    <row r="171" spans="1:25" hidden="1">
       <c r="A171" s="59">
         <v>170</v>
       </c>
@@ -14068,7 +14084,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:25">
+    <row r="172" spans="1:25" hidden="1">
       <c r="A172" s="59">
         <v>171</v>
       </c>
@@ -14099,7 +14115,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="173" spans="1:25">
+    <row r="173" spans="1:25" hidden="1">
       <c r="A173" s="59">
         <v>172</v>
       </c>
@@ -14130,7 +14146,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="174" spans="1:25">
+    <row r="174" spans="1:25" hidden="1">
       <c r="A174" s="59">
         <v>173</v>
       </c>
@@ -14165,7 +14181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:25">
+    <row r="175" spans="1:25" hidden="1">
       <c r="A175" s="59">
         <v>174</v>
       </c>
@@ -14200,7 +14216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:25">
+    <row r="176" spans="1:25" hidden="1">
       <c r="A176" s="59">
         <v>175</v>
       </c>
@@ -14235,7 +14251,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:25">
+    <row r="177" spans="1:25" hidden="1">
       <c r="A177" s="70">
         <v>176</v>
       </c>
@@ -14272,8 +14288,29 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Z1048576">
-    <sortState ref="A21:Z169">
-      <sortCondition descending="1" ref="Y1:Y1048576"/>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="D"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="15">
+      <filters>
+        <filter val="USART1_CK"/>
+        <filter val="USART1_RX"/>
+        <filter val="USART1_TX"/>
+        <filter val="USART2_CK"/>
+        <filter val="USART2_RX"/>
+        <filter val="USART2_TX"/>
+        <filter val="USART3_CK"/>
+        <filter val="USART3_RX"/>
+        <filter val="USART3_TX"/>
+        <filter val="USART6_CK"/>
+        <filter val="USART6_RX"/>
+        <filter val="USART6_TX"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A10:Z41">
+      <sortCondition ref="C1:C1048576"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated "chosen config" column on pin connections sheet These values now match marionette-v1 pin functions
</commit_message>
<xml_diff>
--- a/Marionette_connections.xlsx
+++ b/Marionette_connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="2320" windowWidth="21840" windowHeight="16840" tabRatio="400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8440" windowHeight="17540" tabRatio="400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="264">
   <si>
     <t>Pin number</t>
   </si>
@@ -723,7 +723,100 @@
     <t>x</t>
   </si>
   <si>
-    <t>USART_CK</t>
+    <t>ADC1/2/3_IN2</t>
+  </si>
+  <si>
+    <t>ADC1/2_IN6</t>
+  </si>
+  <si>
+    <t>ADC1/2_IN7</t>
+  </si>
+  <si>
+    <t>SWO</t>
+  </si>
+  <si>
+    <t>ADC1/2/3_IN11</t>
+  </si>
+  <si>
+    <t>ADC1/2/3_IN13</t>
+  </si>
+  <si>
+    <t>ADC1/2_IN14</t>
+  </si>
+  <si>
+    <t>ADC1/2_IN15</t>
+  </si>
+  <si>
+    <t>SDIO_D2-SPI3_SCK</t>
+  </si>
+  <si>
+    <t>SDIO_CK-SPI3_MOSI</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>GPIO - CAN ENABLE</t>
+  </si>
+  <si>
+    <t>ADC3_IN9</t>
+  </si>
+  <si>
+    <t>ADC3_IN14</t>
+  </si>
+  <si>
+    <t>ADC3_IN15</t>
+  </si>
+  <si>
+    <t>ADC3_IN4</t>
+  </si>
+  <si>
+    <t>ADC3_IN5</t>
+  </si>
+  <si>
+    <t>ADC3_IN6</t>
+  </si>
+  <si>
+    <t>ADC3_IN7</t>
+  </si>
+  <si>
+    <t>ADC3_IN8</t>
+  </si>
+  <si>
+    <t>GPIO - LED3</t>
+  </si>
+  <si>
+    <t>GPIO - LED4</t>
+  </si>
+  <si>
+    <t>GPIO - LED5</t>
+  </si>
+  <si>
+    <t>GPIO - LED6</t>
+  </si>
+  <si>
+    <t>GPIO - LED7</t>
+  </si>
+  <si>
+    <t>GPIO - LED8</t>
+  </si>
+  <si>
+    <t>GPIO - LED9</t>
+  </si>
+  <si>
+    <t>GPIO - SDIO_PWR</t>
+  </si>
+  <si>
+    <t>I2C1_SCL - mBUS</t>
+  </si>
+  <si>
+    <t>I2C1_SDA - mBUS</t>
+  </si>
+  <si>
+    <t>GPIO - ULPI_!RST_B</t>
+  </si>
+  <si>
+    <t>GPIO - SD_DETECT</t>
   </si>
 </sst>
 </file>
@@ -783,7 +876,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -860,12 +953,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF93CDDD"/>
         <bgColor rgb="FFB9CDE5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1158,7 +1245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1434,10 +1521,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2023,8 +2106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6679,10 +6762,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK177"/>
   <sheetViews>
-    <sheetView topLeftCell="A1048576" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1048576" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="660" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="C1:Y1048576"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection activeCell="D1048576" sqref="D1:X1048576"/>
+      <selection pane="bottomLeft" activeCell="Y42" sqref="Y42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6690,9 +6773,9 @@
     <col min="1" max="1" width="8.83203125" style="32"/>
     <col min="2" max="2" width="8.83203125" style="33" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="34" customWidth="1"/>
-    <col min="5" max="22" width="8.83203125" style="32" customWidth="1"/>
-    <col min="23" max="24" width="8.83203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="34" hidden="1" customWidth="1"/>
+    <col min="5" max="22" width="8.83203125" style="32" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="8.83203125" style="34" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="15.5" style="32" bestFit="1" customWidth="1"/>
     <col min="26" max="1025" width="8.83203125" style="32"/>
   </cols>
@@ -7816,7 +7899,7 @@
       </c>
       <c r="W2" s="55"/>
       <c r="X2" s="56"/>
-      <c r="Y2" s="98" t="s">
+      <c r="Y2" s="97" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7911,7 +7994,7 @@
       <c r="W4" s="61"/>
       <c r="X4" s="62"/>
       <c r="Y4" s="75" t="s">
-        <v>9</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:1024" s="57" customFormat="1">
@@ -8091,7 +8174,7 @@
       <c r="W8" s="61"/>
       <c r="X8" s="62"/>
       <c r="Y8" s="75" t="s">
-        <v>6</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:1024" s="57" customFormat="1">
@@ -8136,7 +8219,7 @@
       <c r="W9" s="61"/>
       <c r="X9" s="62"/>
       <c r="Y9" s="75" t="s">
-        <v>6</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:1024" s="57" customFormat="1">
@@ -8256,8 +8339,8 @@
       <c r="V12" s="61"/>
       <c r="W12" s="61"/>
       <c r="X12" s="62"/>
-      <c r="Y12" s="81" t="s">
-        <v>39</v>
+      <c r="Y12" s="96" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:1024" s="57" customFormat="1">
@@ -8616,7 +8699,7 @@
       <c r="W21" s="61"/>
       <c r="X21" s="62"/>
       <c r="Y21" s="67" t="s">
-        <v>18</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:25" s="57" customFormat="1">
@@ -8657,7 +8740,7 @@
       <c r="W22" s="61"/>
       <c r="X22" s="62"/>
       <c r="Y22" s="67" t="s">
-        <v>18</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:25" s="57" customFormat="1">
@@ -8745,7 +8828,7 @@
       <c r="W24" s="61"/>
       <c r="X24" s="62"/>
       <c r="Y24" s="74" t="s">
-        <v>22</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:25" s="57" customFormat="1">
@@ -8784,7 +8867,7 @@
       <c r="W25" s="61"/>
       <c r="X25" s="62"/>
       <c r="Y25" s="74" t="s">
-        <v>23</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:25" s="57" customFormat="1">
@@ -9224,7 +9307,7 @@
       <c r="W35" s="61"/>
       <c r="X35" s="62"/>
       <c r="Y35" s="75" t="s">
-        <v>6</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="57" customFormat="1">
@@ -9318,7 +9401,7 @@
       <c r="W37" s="61"/>
       <c r="X37" s="62"/>
       <c r="Y37" s="75" t="s">
-        <v>6</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:25" s="57" customFormat="1">
@@ -9361,7 +9444,7 @@
       <c r="W38" s="61"/>
       <c r="X38" s="62"/>
       <c r="Y38" s="75" t="s">
-        <v>6</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:25" s="57" customFormat="1">
@@ -9404,7 +9487,7 @@
       <c r="W39" s="61"/>
       <c r="X39" s="62"/>
       <c r="Y39" s="75" t="s">
-        <v>6</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:25" s="57" customFormat="1">
@@ -9482,7 +9565,7 @@
       <c r="W41" s="61"/>
       <c r="X41" s="62"/>
       <c r="Y41" s="96" t="s">
-        <v>18</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:25" s="57" customFormat="1">
@@ -9605,7 +9688,7 @@
       <c r="W44" s="61"/>
       <c r="X44" s="62"/>
       <c r="Y44" s="80" t="s">
-        <v>75</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:25" s="57" customFormat="1">
@@ -9691,7 +9774,7 @@
       <c r="W46" s="61"/>
       <c r="X46" s="62"/>
       <c r="Y46" s="80" t="s">
-        <v>67</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:25" s="57" customFormat="1">
@@ -9726,7 +9809,7 @@
       <c r="W47" s="61"/>
       <c r="X47" s="62"/>
       <c r="Y47" s="67" t="s">
-        <v>34</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:25" s="57" customFormat="1">
@@ -9761,7 +9844,7 @@
       <c r="W48" s="61"/>
       <c r="X48" s="62"/>
       <c r="Y48" s="67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:26" s="57" customFormat="1">
@@ -9796,7 +9879,7 @@
       <c r="W49" s="72"/>
       <c r="X49" s="73"/>
       <c r="Y49" s="67" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:26" s="57" customFormat="1">
@@ -10025,8 +10108,8 @@
       <c r="V55" s="61"/>
       <c r="W55" s="61"/>
       <c r="X55" s="62"/>
-      <c r="Y55" s="97" t="s">
-        <v>154</v>
+      <c r="Y55" s="96" t="s">
+        <v>242</v>
       </c>
       <c r="Z55" s="57" t="s">
         <v>231</v>
@@ -10065,8 +10148,8 @@
       <c r="V56" s="61"/>
       <c r="W56" s="61"/>
       <c r="X56" s="62"/>
-      <c r="Y56" s="97" t="s">
-        <v>156</v>
+      <c r="Y56" s="96" t="s">
+        <v>18</v>
       </c>
       <c r="Z56" s="57" t="s">
         <v>231</v>
@@ -10105,8 +10188,8 @@
       <c r="V57" s="61"/>
       <c r="W57" s="61"/>
       <c r="X57" s="62"/>
-      <c r="Y57" s="97" t="s">
-        <v>232</v>
+      <c r="Y57" s="96" t="s">
+        <v>18</v>
       </c>
       <c r="Z57" s="57" t="s">
         <v>231</v>
@@ -11086,8 +11169,8 @@
       <c r="V84" s="61"/>
       <c r="W84" s="61"/>
       <c r="X84" s="62"/>
-      <c r="Y84" s="74" t="s">
-        <v>26</v>
+      <c r="Y84" s="96" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:25">
@@ -11124,7 +11207,7 @@
       <c r="W85" s="61"/>
       <c r="X85" s="62"/>
       <c r="Y85" s="75" t="s">
-        <v>10</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:25">
@@ -11161,7 +11244,7 @@
       <c r="W86" s="61"/>
       <c r="X86" s="62"/>
       <c r="Y86" s="75" t="s">
-        <v>10</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:25">
@@ -11198,7 +11281,7 @@
       <c r="W87" s="61"/>
       <c r="X87" s="62"/>
       <c r="Y87" s="75" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:25">
@@ -11235,7 +11318,7 @@
       <c r="W88" s="61"/>
       <c r="X88" s="62"/>
       <c r="Y88" s="75" t="s">
-        <v>10</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:25">
@@ -11272,7 +11355,7 @@
       <c r="W89" s="61"/>
       <c r="X89" s="62"/>
       <c r="Y89" s="75" t="s">
-        <v>10</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:25">
@@ -11309,7 +11392,7 @@
       <c r="W90" s="61"/>
       <c r="X90" s="62"/>
       <c r="Y90" s="75" t="s">
-        <v>10</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:25">
@@ -11346,7 +11429,7 @@
       <c r="W91" s="61"/>
       <c r="X91" s="62"/>
       <c r="Y91" s="75" t="s">
-        <v>10</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:25">
@@ -11383,7 +11466,7 @@
       <c r="W92" s="61"/>
       <c r="X92" s="62"/>
       <c r="Y92" s="75" t="s">
-        <v>10</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:25">
@@ -11916,7 +11999,7 @@
       <c r="W107" s="61"/>
       <c r="X107" s="62"/>
       <c r="Y107" s="63" t="s">
-        <v>18</v>
+        <v>252</v>
       </c>
     </row>
     <row r="108" spans="1:25">
@@ -11951,7 +12034,7 @@
       <c r="W108" s="61"/>
       <c r="X108" s="62"/>
       <c r="Y108" s="67" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
     </row>
     <row r="109" spans="1:25">
@@ -11989,8 +12072,8 @@
       <c r="V109" s="61"/>
       <c r="W109" s="61"/>
       <c r="X109" s="62"/>
-      <c r="Y109" s="63" t="s">
-        <v>18</v>
+      <c r="Y109" s="67" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="110" spans="1:25">
@@ -12027,7 +12110,7 @@
       <c r="W110" s="61"/>
       <c r="X110" s="62"/>
       <c r="Y110" s="67" t="s">
-        <v>18</v>
+        <v>255</v>
       </c>
     </row>
     <row r="111" spans="1:25">
@@ -12068,7 +12151,7 @@
       <c r="W111" s="61"/>
       <c r="X111" s="62"/>
       <c r="Y111" s="67" t="s">
-        <v>18</v>
+        <v>256</v>
       </c>
     </row>
     <row r="112" spans="1:25">
@@ -12109,7 +12192,7 @@
       <c r="W112" s="61"/>
       <c r="X112" s="62"/>
       <c r="Y112" s="67" t="s">
-        <v>18</v>
+        <v>257</v>
       </c>
     </row>
     <row r="113" spans="1:25">
@@ -12145,8 +12228,8 @@
       <c r="V113" s="72"/>
       <c r="W113" s="72"/>
       <c r="X113" s="73"/>
-      <c r="Y113" s="63" t="s">
-        <v>18</v>
+      <c r="Y113" s="67" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:25">
@@ -12517,8 +12600,8 @@
       <c r="V123" s="61"/>
       <c r="W123" s="61"/>
       <c r="X123" s="62"/>
-      <c r="Y123" s="74" t="s">
-        <v>29</v>
+      <c r="Y123" s="96" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="124" spans="1:25">
@@ -13127,7 +13210,7 @@
       <c r="W140" s="61"/>
       <c r="X140" s="62"/>
       <c r="Y140" s="67" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
     </row>
     <row r="141" spans="1:25">

</xml_diff>

<commit_message>
Updated chosen config pin labels
</commit_message>
<xml_diff>
--- a/Marionette_connections.xlsx
+++ b/Marionette_connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8440" windowHeight="17540" tabRatio="400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="17560" tabRatio="400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="269">
   <si>
     <t>Pin number</t>
   </si>
@@ -817,6 +817,21 @@
   </si>
   <si>
     <t>GPIO - SD_DETECT</t>
+  </si>
+  <si>
+    <t>SDIO_D3-SPI3_MISO</t>
+  </si>
+  <si>
+    <t>GPIO - LED2</t>
+  </si>
+  <si>
+    <t>GPIO - LED1_R</t>
+  </si>
+  <si>
+    <t>GPIO - LED1_G</t>
+  </si>
+  <si>
+    <t>GPIO - LED1_B</t>
   </si>
 </sst>
 </file>
@@ -6762,10 +6777,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048576" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="660" activePane="bottomLeft"/>
-      <selection activeCell="D1048576" sqref="D1:X1048576"/>
-      <selection pane="bottomLeft" activeCell="Y42" sqref="Y42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="660" topLeftCell="A115" activePane="bottomLeft"/>
+      <selection activeCell="D2" sqref="D1:K1048576"/>
+      <selection pane="bottomLeft" activeCell="Y66" sqref="Y66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9179,7 +9194,7 @@
       <c r="V32" s="61"/>
       <c r="W32" s="61"/>
       <c r="X32" s="62"/>
-      <c r="Y32" s="63" t="s">
+      <c r="Y32" s="67" t="s">
         <v>18</v>
       </c>
     </row>
@@ -9731,7 +9746,7 @@
       <c r="W45" s="61"/>
       <c r="X45" s="62"/>
       <c r="Y45" s="80" t="s">
-        <v>77</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="57" customFormat="1">
@@ -10189,7 +10204,7 @@
       <c r="W57" s="61"/>
       <c r="X57" s="62"/>
       <c r="Y57" s="96" t="s">
-        <v>18</v>
+        <v>265</v>
       </c>
       <c r="Z57" s="57" t="s">
         <v>231</v>
@@ -10427,7 +10442,7 @@
       <c r="W63" s="61"/>
       <c r="X63" s="62"/>
       <c r="Y63" s="67" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:26">
@@ -10462,7 +10477,7 @@
       <c r="W64" s="61"/>
       <c r="X64" s="62"/>
       <c r="Y64" s="67" t="s">
-        <v>18</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:25">
@@ -10497,7 +10512,7 @@
       <c r="W65" s="72"/>
       <c r="X65" s="73"/>
       <c r="Y65" s="67" t="s">
-        <v>18</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:25">
@@ -11570,7 +11585,7 @@
       <c r="V95" s="61"/>
       <c r="W95" s="61"/>
       <c r="X95" s="62"/>
-      <c r="Y95" s="63" t="s">
+      <c r="Y95" s="67" t="s">
         <v>18</v>
       </c>
     </row>
@@ -11605,7 +11620,7 @@
       <c r="V96" s="61"/>
       <c r="W96" s="61"/>
       <c r="X96" s="62"/>
-      <c r="Y96" s="63" t="s">
+      <c r="Y96" s="67" t="s">
         <v>18</v>
       </c>
     </row>
@@ -11675,7 +11690,7 @@
       <c r="V98" s="55"/>
       <c r="W98" s="55"/>
       <c r="X98" s="56"/>
-      <c r="Y98" s="63" t="s">
+      <c r="Y98" s="67" t="s">
         <v>18</v>
       </c>
     </row>
@@ -11745,7 +11760,7 @@
       <c r="V100" s="61"/>
       <c r="W100" s="61"/>
       <c r="X100" s="62"/>
-      <c r="Y100" s="63" t="s">
+      <c r="Y100" s="67" t="s">
         <v>18</v>
       </c>
     </row>
@@ -11922,7 +11937,7 @@
       <c r="V105" s="61"/>
       <c r="W105" s="61"/>
       <c r="X105" s="62"/>
-      <c r="Y105" s="63" t="s">
+      <c r="Y105" s="67" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>